<commit_message>
more work on by waters data
</commit_message>
<xml_diff>
--- a/data/landings/cdfw/public/fish_bulletins/raw/fb144/raw/Table7.xlsx
+++ b/data/landings/cdfw/public/fish_bulletins/raw/fb144/raw/Table7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/wc_cc_synthesis/data/landings/cdfw/public/fish_bulletins/raw/fb144/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2046EB92-EEE5-1044-94AF-0EDEF7B08158}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F09FE12A-863B-9C44-9E89-9308EAA0AA79}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="26080" yWindow="820" windowWidth="18600" windowHeight="25080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="80">
   <si>
     <t>Species</t>
   </si>
@@ -34,15 +34,6 @@
     <t>—</t>
   </si>
   <si>
-    <t>•202,513</t>
-  </si>
-  <si>
-    <t>2:10,604</t>
-  </si>
-  <si>
-    <t>2,5%,118</t>
-  </si>
-  <si>
     <t>Crustacean:</t>
   </si>
   <si>
@@ -85,9 +76,6 @@
     <t>Croaker, white</t>
   </si>
   <si>
-    <t>496, 17</t>
-  </si>
-  <si>
     <t>Flounder</t>
   </si>
   <si>
@@ -197,9 +185,6 @@
   </si>
   <si>
     <t>Tuna, blucfin</t>
-  </si>
-  <si>
-    <t>114U5SttX)</t>
   </si>
   <si>
     <t>T urbot</t>
@@ -640,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -662,28 +647,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="F1" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="H1" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -693,13 +678,13 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2">
-        <v>60609377</v>
+        <v>69609377</v>
       </c>
       <c r="E3" s="2">
-        <v>60609377</v>
+        <v>69609377</v>
       </c>
       <c r="F3" s="3">
         <f>E3-SUM(B3:D3)</f>
@@ -710,12 +695,12 @@
       </c>
       <c r="I3" s="3">
         <f>H3-SUM(G3,B3:D3)</f>
-        <v>9000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B4" s="2">
         <v>281224</v>
@@ -724,11 +709,11 @@
         <v>31960</v>
       </c>
       <c r="E4" s="2">
-        <v>313181</v>
+        <v>313184</v>
       </c>
       <c r="F4" s="3">
         <f t="shared" ref="F4:F67" si="0">E4-SUM(B4:D4)</f>
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="H4" s="2">
         <v>313184</v>
@@ -740,7 +725,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B5" s="2">
         <v>7620</v>
@@ -753,16 +738,16 @@
         <v>0</v>
       </c>
       <c r="H5" s="2">
-        <v>762</v>
+        <v>7620</v>
       </c>
       <c r="I5" s="3">
         <f t="shared" si="1"/>
-        <v>-6858</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B6" s="2">
         <v>17841537</v>
@@ -787,7 +772,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B7" s="2">
         <v>14284</v>
@@ -796,11 +781,11 @@
         <v>3</v>
       </c>
       <c r="E7" s="2">
-        <v>14281</v>
+        <v>14284</v>
       </c>
       <c r="F7" s="3">
         <f t="shared" si="0"/>
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>3</v>
@@ -815,13 +800,13 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B8" s="2">
-        <v>318531</v>
+        <v>348531</v>
       </c>
       <c r="E8" s="2">
-        <v>318531</v>
+        <v>348531</v>
       </c>
       <c r="F8" s="3">
         <f t="shared" si="0"/>
@@ -832,12 +817,12 @@
       </c>
       <c r="I8" s="3">
         <f t="shared" si="1"/>
-        <v>30000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B9" s="2">
         <v>496378</v>
@@ -845,24 +830,24 @@
       <c r="D9" s="2">
         <v>39</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+      <c r="E9" s="2">
+        <v>496417</v>
+      </c>
+      <c r="F9" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="H9" s="2">
-        <v>196417</v>
+        <v>496417</v>
       </c>
       <c r="I9" s="3">
         <f t="shared" si="1"/>
-        <v>-300000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B10" s="2">
         <v>860634</v>
@@ -887,7 +872,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B11" s="2">
         <v>6041</v>
@@ -909,7 +894,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B12" s="2">
         <v>45194</v>
@@ -934,7 +919,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D13" s="2">
         <v>190199</v>
@@ -956,29 +941,29 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B14" s="2">
         <v>14430</v>
       </c>
       <c r="E14" s="2">
-        <v>11430</v>
+        <v>14430</v>
       </c>
       <c r="F14" s="3">
         <f t="shared" si="0"/>
-        <v>-3000</v>
+        <v>0</v>
       </c>
       <c r="H14" s="2">
-        <v>11130</v>
+        <v>14430</v>
       </c>
       <c r="I14" s="3">
         <f t="shared" si="1"/>
-        <v>-3300</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B15" s="2">
         <v>25431</v>
@@ -1000,10 +985,10 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B16" s="2">
-        <v>821919</v>
+        <v>824919</v>
       </c>
       <c r="D16" s="2">
         <v>13139</v>
@@ -1013,19 +998,19 @@
       </c>
       <c r="F16" s="3">
         <f t="shared" si="0"/>
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="H16" s="2">
         <v>838058</v>
       </c>
       <c r="I16" s="3">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B17" s="2">
         <v>498</v>
@@ -1047,7 +1032,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B18" s="2">
         <v>218604</v>
@@ -1060,16 +1045,16 @@
         <v>0</v>
       </c>
       <c r="H18" s="2">
-        <v>218601</v>
+        <v>218604</v>
       </c>
       <c r="I18" s="3">
         <f t="shared" si="1"/>
-        <v>-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B19" s="2">
         <v>271902</v>
@@ -1091,7 +1076,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B20" s="2">
         <v>13317</v>
@@ -1113,7 +1098,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B21" s="2">
         <v>921968</v>
@@ -1138,7 +1123,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B22" s="2">
         <v>13400</v>
@@ -1166,29 +1151,29 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B23" s="2">
-        <v>38180517</v>
+        <v>38180547</v>
       </c>
       <c r="E23" s="2">
         <v>38180547</v>
       </c>
       <c r="F23" s="3">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="H23" s="2">
         <v>38180547</v>
       </c>
       <c r="I23" s="3">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B24" s="2">
         <v>1166607</v>
@@ -1210,7 +1195,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B25" s="2">
         <v>17298</v>
@@ -1232,7 +1217,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B26" s="2">
         <v>201728</v>
@@ -1240,12 +1225,12 @@
       <c r="D26" s="2">
         <v>785</v>
       </c>
-      <c r="E26" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F26" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+      <c r="E26" s="2">
+        <v>202513</v>
+      </c>
+      <c r="F26" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="H26" s="2">
         <v>202513</v>
@@ -1257,7 +1242,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B27" s="2">
         <v>111593</v>
@@ -1282,7 +1267,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B28" s="2">
         <v>9589787</v>
@@ -1310,7 +1295,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B29" s="2">
         <v>3768959</v>
@@ -1335,7 +1320,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B30" s="2">
         <v>7401591</v>
@@ -1344,11 +1329,11 @@
         <v>138</v>
       </c>
       <c r="E30" s="2">
-        <v>7101729</v>
+        <v>7401729</v>
       </c>
       <c r="F30" s="3">
         <f t="shared" si="0"/>
-        <v>-300000</v>
+        <v>0</v>
       </c>
       <c r="H30" s="2">
         <v>7401729</v>
@@ -1360,7 +1345,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B31" s="2">
         <v>685402</v>
@@ -1388,7 +1373,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B32" s="2">
         <v>148766</v>
@@ -1410,7 +1395,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B33" s="2">
         <v>56045</v>
@@ -1435,7 +1420,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B34" s="2">
         <v>11893</v>
@@ -1443,24 +1428,24 @@
       <c r="D34" s="2">
         <v>218711</v>
       </c>
-      <c r="E34" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F34" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+      <c r="E34" s="2">
+        <v>230604</v>
+      </c>
+      <c r="F34" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="H34" s="2">
-        <v>230601</v>
+        <v>230604</v>
       </c>
       <c r="I34" s="3">
         <f t="shared" si="1"/>
-        <v>-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B35" s="2">
         <v>507588</v>
@@ -1485,7 +1470,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B36" s="2">
         <v>586249</v>
@@ -1494,11 +1479,11 @@
         <v>10649</v>
       </c>
       <c r="E36" s="2">
-        <v>596888</v>
+        <v>596898</v>
       </c>
       <c r="F36" s="3">
         <f t="shared" si="0"/>
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="H36" s="2">
         <v>596898</v>
@@ -1510,7 +1495,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B37" s="2">
         <v>18605</v>
@@ -1538,7 +1523,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B38" s="2">
         <v>196751</v>
@@ -1560,7 +1545,7 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B39" s="2">
         <v>591975</v>
@@ -1582,7 +1567,7 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B40" s="2">
         <v>199694</v>
@@ -1604,7 +1589,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B41" s="2">
         <v>6814501</v>
@@ -1629,7 +1614,7 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B42" s="2">
         <v>5757762</v>
@@ -1657,7 +1642,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B43" s="2">
         <v>2733760</v>
@@ -1682,10 +1667,10 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B44" s="2">
-        <v>1750519</v>
+        <v>1750549</v>
       </c>
       <c r="C44" s="2">
         <v>15489</v>
@@ -1695,19 +1680,19 @@
       </c>
       <c r="F44" s="3">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="H44" s="2">
         <v>1766038</v>
       </c>
       <c r="I44" s="3">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B45" s="2">
         <v>305405</v>
@@ -1732,7 +1717,7 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B46" s="2">
         <v>31712</v>
@@ -1754,7 +1739,7 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B47" s="2">
         <v>303467</v>
@@ -1779,7 +1764,7 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B48" s="2">
         <v>15184473</v>
@@ -1810,7 +1795,7 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B49" s="2">
         <v>4229</v>
@@ -1838,7 +1823,7 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B50" s="2">
         <v>1791634</v>
@@ -1866,7 +1851,7 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B51" s="2">
         <v>116902</v>
@@ -1884,17 +1869,17 @@
       <c r="G51" s="2">
         <v>4002499</v>
       </c>
-      <c r="H51" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="I51" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+      <c r="H51" s="2">
+        <v>114958800</v>
+      </c>
+      <c r="I51" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>3</v>
@@ -1922,7 +1907,7 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B53" s="2">
         <v>72747</v>
@@ -1947,7 +1932,7 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D54" s="2">
         <v>982</v>
@@ -1969,7 +1954,7 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B55" s="2">
         <v>170</v>
@@ -1994,7 +1979,7 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B56" s="2">
         <v>13179</v>
@@ -2019,7 +2004,7 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B57" s="2">
         <v>1776</v>
@@ -2044,7 +2029,7 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B58" s="2">
         <v>2526296</v>
@@ -2059,17 +2044,17 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H58" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I58" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+      <c r="H58" s="2">
+        <v>2596118</v>
+      </c>
+      <c r="I58" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F59" s="3">
         <f t="shared" si="0"/>
@@ -2082,7 +2067,7 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B60" s="2">
         <v>11716488</v>
@@ -2104,7 +2089,7 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B61" s="2">
         <v>324386</v>
@@ -2126,7 +2111,7 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B62" s="2">
         <v>449874</v>
@@ -2135,23 +2120,23 @@
         <v>10</v>
       </c>
       <c r="E62" s="2">
-        <v>449881</v>
+        <v>449884</v>
       </c>
       <c r="F62" s="3">
         <f t="shared" si="0"/>
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="H62" s="2">
-        <v>419884</v>
+        <v>449884</v>
       </c>
       <c r="I62" s="3">
         <f t="shared" si="1"/>
-        <v>-30000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B63" s="2">
         <v>2590</v>
@@ -2173,7 +2158,7 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B64" s="2">
         <v>423</v>
@@ -2195,7 +2180,7 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B65" s="2">
         <v>19771</v>
@@ -2217,7 +2202,7 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B66" s="2">
         <v>1408453</v>
@@ -2245,7 +2230,7 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F67" s="3">
         <f t="shared" si="0"/>
@@ -2258,7 +2243,7 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B68" s="2">
         <v>4421581</v>
@@ -2280,7 +2265,7 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B69" s="2">
         <v>2532</v>
@@ -2302,29 +2287,29 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B70" s="2">
-        <v>9191</v>
+        <v>9194</v>
       </c>
       <c r="E70" s="2">
         <v>9194</v>
       </c>
       <c r="F70" s="3">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H70" s="2">
         <v>9194</v>
       </c>
       <c r="I70" s="3">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B71" s="2">
         <v>12710</v>
@@ -2346,7 +2331,7 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B72" s="2">
         <v>729431</v>
@@ -2368,7 +2353,7 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B73" s="2">
         <v>19601922</v>
@@ -2430,11 +2415,11 @@
     </row>
     <row r="75" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B75" s="3">
         <f>B74-SUM(B2:B73)</f>
-        <v>9033063</v>
+        <v>0</v>
       </c>
       <c r="C75" s="3">
         <f t="shared" ref="C75:I75" si="4">C74-SUM(C2:C73)</f>
@@ -2446,11 +2431,11 @@
       </c>
       <c r="E75" s="3">
         <f t="shared" si="4"/>
-        <v>10262553</v>
-      </c>
-      <c r="F75" s="3" t="e">
+        <v>0</v>
+      </c>
+      <c r="F75" s="3">
         <f t="shared" si="4"/>
-        <v>#VALUE!</v>
+        <v>0</v>
       </c>
       <c r="G75" s="3">
         <f t="shared" si="4"/>
@@ -2458,11 +2443,11 @@
       </c>
       <c r="H75" s="3">
         <f t="shared" si="4"/>
-        <v>117895082</v>
-      </c>
-      <c r="I75" s="3" t="e">
+        <v>0</v>
+      </c>
+      <c r="I75" s="3">
         <f t="shared" si="4"/>
-        <v>#VALUE!</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>